<commit_message>
Fixed Data Set Sample
</commit_message>
<xml_diff>
--- a/Data Sample.xlsx
+++ b/Data Sample.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ali_A\Webdata\NBA_Player_Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{619DE03F-92FE-4DA1-8E12-4626E62EF951}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFD6D91-ACC9-48E5-A8E1-A06B4616489A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{013B66EF-09E7-45CD-9B43-C851E42C786E}"/>
   </bookViews>
@@ -39,12 +39,6 @@
     <t>Year in League</t>
   </si>
   <si>
-    <t>Height</t>
-  </si>
-  <si>
-    <t>Weight</t>
-  </si>
-  <si>
     <t>Tm</t>
   </si>
   <si>
@@ -60,9 +54,6 @@
     <t>TS%</t>
   </si>
   <si>
-    <t>3PAr</t>
-  </si>
-  <si>
     <t>FTr</t>
   </si>
   <si>
@@ -208,6 +199,15 @@
   </si>
   <si>
     <t>TOT</t>
+  </si>
+  <si>
+    <t>Height(CM)</t>
+  </si>
+  <si>
+    <t>Weight(KG)</t>
+  </si>
+  <si>
+    <t>git status</t>
   </si>
 </sst>
 </file>
@@ -243,9 +243,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -560,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DEBA307-7004-4218-BFFD-DCEFB0352AFB}">
-  <dimension ref="A1:AY6"/>
+  <dimension ref="A1:AY14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,145 +581,142 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>41</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>42</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>43</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>44</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>45</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>46</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>47</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
@@ -728,7 +724,7 @@
         <v>2003</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C2">
         <v>28</v>
@@ -736,14 +732,14 @@
       <c r="D2">
         <v>6</v>
       </c>
-      <c r="E2" s="1">
-        <v>44353</v>
+      <c r="E2">
+        <v>198</v>
       </c>
       <c r="F2">
-        <v>223</v>
+        <v>101</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="H2">
         <v>14</v>
@@ -883,7 +879,7 @@
         <v>2003</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C3">
         <v>26</v>
@@ -891,14 +887,14 @@
       <c r="D3">
         <v>7</v>
       </c>
-      <c r="E3" s="1">
-        <v>44356</v>
+      <c r="E3">
+        <v>206</v>
       </c>
       <c r="F3">
-        <v>225</v>
+        <v>102</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="H3">
         <v>81</v>
@@ -1038,7 +1034,7 @@
         <v>2003</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C4">
         <v>25</v>
@@ -1046,14 +1042,14 @@
       <c r="D4">
         <v>8</v>
       </c>
-      <c r="E4" s="1">
-        <v>44348</v>
+      <c r="E4">
+        <v>185</v>
       </c>
       <c r="F4">
-        <v>185</v>
+        <v>83</v>
       </c>
       <c r="G4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H4">
         <v>66</v>
@@ -1193,7 +1189,7 @@
         <v>2003</v>
       </c>
       <c r="B5" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C5">
         <v>24</v>
@@ -1201,14 +1197,14 @@
       <c r="D5">
         <v>2</v>
       </c>
-      <c r="E5" s="1">
-        <v>44357</v>
+      <c r="E5">
+        <v>208</v>
       </c>
       <c r="F5">
-        <v>255</v>
+        <v>115</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H5">
         <v>80</v>
@@ -1348,7 +1344,7 @@
         <v>2003</v>
       </c>
       <c r="B6" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C6">
         <v>27</v>
@@ -1356,14 +1352,14 @@
       <c r="D6">
         <v>7</v>
       </c>
-      <c r="E6" s="1">
-        <v>44352</v>
+      <c r="E6">
+        <v>203</v>
       </c>
       <c r="F6">
-        <v>205</v>
+        <v>99</v>
       </c>
       <c r="G6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="H6">
         <v>76</v>
@@ -1496,6 +1492,11 @@
       </c>
       <c r="AY6">
         <v>1713</v>
+      </c>
+    </row>
+    <row r="14" spans="1:51" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>